<commit_message>
Add result for Nr 2
</commit_message>
<xml_diff>
--- a/src/uebung5/TemplateTestCase v1.6.xlsx
+++ b/src/uebung5/TemplateTestCase v1.6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Data\eclipse-uni-workspace\Prog2\Software-Engineering\src\uebung5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58212AC7-F3ED-48DF-B4D9-0F4A6AC5D682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99049446-CB2F-449D-A773-ABF611FAF51D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
   <si>
     <t>Testprozedur:</t>
   </si>
@@ -295,9 +295,6 @@
 E-Mail-Adresse: max.mustermann@example.com</t>
   </si>
   <si>
-    <t xml:space="preserve">SYSTEM </t>
-  </si>
-  <si>
     <t>Benutzer lädt seine Bewerbungsmappe als PDF hoch
 Datei: BewerbungsMappeMax.pdf</t>
   </si>
@@ -328,6 +325,12 @@
   </si>
   <si>
     <t>U1 hat einen neuen Bewerber</t>
+  </si>
+  <si>
+    <t>SYSTEM akzeptiert die vom Akteur eingegebenen Werte</t>
+  </si>
+  <si>
+    <t>Werte wurden akzeptiert</t>
   </si>
 </sst>
 </file>
@@ -801,6 +804,51 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -810,51 +858,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1163,20 +1166,20 @@
       <c r="C4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="40"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="55"/>
     </row>
     <row r="5" spans="3:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="16"/>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="34"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="36" t="s">
+      <c r="C6" s="49"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="37"/>
+      <c r="F6" s="52"/>
     </row>
     <row r="7" spans="3:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="21" t="s">
@@ -1308,7 +1311,7 @@
   <dimension ref="B1:G30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="142" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1396,173 +1399,175 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:7" s="46" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="41">
+    <row r="11" spans="2:7" s="39" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="34">
         <v>1</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="43" t="s">
+      <c r="E11" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="44" t="s">
+      <c r="F11" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="45"/>
-    </row>
-    <row r="12" spans="2:7" s="46" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="41">
+      <c r="G11" s="38"/>
+    </row>
+    <row r="12" spans="2:7" s="39" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="34">
         <v>2</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E12" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="44" t="s">
+      <c r="F12" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="45"/>
+      <c r="G12" s="38"/>
     </row>
     <row r="13" spans="2:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="41">
+      <c r="B13" s="34">
         <v>3</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="38"/>
+    </row>
+    <row r="14" spans="2:7" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="B14" s="34">
+        <v>4</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="38"/>
+    </row>
+    <row r="15" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B15" s="34">
+        <v>5</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="38"/>
+    </row>
+    <row r="16" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B16" s="34">
+        <v>6</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="38"/>
+    </row>
+    <row r="17" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B17" s="34">
+        <v>7</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="44" t="s">
+      <c r="E17" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="45"/>
-    </row>
-    <row r="14" spans="2:7" ht="173.25" x14ac:dyDescent="0.25">
-      <c r="B14" s="41">
-        <v>4</v>
-      </c>
-      <c r="C14" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="43"/>
-      <c r="F14" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="45"/>
-    </row>
-    <row r="15" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B15" s="41">
-        <v>5</v>
-      </c>
-      <c r="C15" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" s="45"/>
-    </row>
-    <row r="16" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="41">
+      <c r="G17" s="38"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="40"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="38"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="40"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="38"/>
+    </row>
+    <row r="20" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="41"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="45"/>
+    </row>
+    <row r="21" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="39"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="42" t="s">
+      <c r="F21" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" s="45"/>
-    </row>
-    <row r="17" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B17" s="41">
-        <v>7</v>
-      </c>
-      <c r="C17" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="45"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="47"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="45"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="47"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="45"/>
-    </row>
-    <row r="20" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="48"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="52"/>
-    </row>
-    <row r="21" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="46"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="54" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="G21" s="46"/>
+      <c r="G21" s="39"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="46"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C25" s="16" t="s">

</xml_diff>